<commit_message>
Merged the Admin code and code restructure of the Triner.
</commit_message>
<xml_diff>
--- a/IctakTechBlog/src/main/resources/TestData.xlsx
+++ b/IctakTechBlog/src/main/resources/TestData.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhPJ/19L8BctuRFdOeBOhzhdUQDcQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhzZ7keGwLMdW9VgM8sHuWi1OCJXw=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>trainerict@gmail.com</t>
   </si>
@@ -27,22 +27,25 @@
     <t>xyz</t>
   </si>
   <si>
-    <t>PriyaNavya</t>
-  </si>
-  <si>
-    <t>priyanavya@gmail.com</t>
-  </si>
-  <si>
-    <t>Testnavya1</t>
-  </si>
-  <si>
-    <t>Priyatesting</t>
-  </si>
-  <si>
-    <t>priyatesting@gmail.com</t>
-  </si>
-  <si>
-    <t>Priyatestin1</t>
+    <t>hjjk</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>PriyaNavyatesting</t>
+  </si>
+  <si>
+    <t>priyanavyate@gmail.com</t>
+  </si>
+  <si>
+    <t>Testnavya1234</t>
+  </si>
+  <si>
+    <t>Priya</t>
+  </si>
+  <si>
+    <t>asd</t>
   </si>
   <si>
     <t>Moon bound rocket</t>
@@ -54,6 +57,9 @@
     <t>A rocket stage expected to impact the moon is still most likely to belong to China’s 2014 moon mission, despite a denial from the country’s Ministry of Foreign Affairs.</t>
   </si>
   <si>
+    <t>A rocket stage expected to impact the moon is still most likely to belong to China’s 2014 moon mission, despite a denial from the country’s Ministry of Foreign Affairs. Updated</t>
+  </si>
+  <si>
     <t>NASA's NuSTAR makes illuminating discoveries with 'nuisance' light</t>
   </si>
   <si>
@@ -63,12 +69,18 @@
     <t>For almost 10 years, NASA's NuSTAR (Nuclear Spectroscopic Telescope Array) X-ray space observatory has been studying some of the highest-energy objects in the universe, such as colliding dead stars and enormous black holes feasting on hot gas. During that time, scientists have had to deal with stray light leaking in through the sides of the observatory, which can interfere with observations much like external noise can drown out a phone call.</t>
   </si>
   <si>
+    <t xml:space="preserve">NASA's NuSTAR </t>
+  </si>
+  <si>
+    <t>https://scx1.b-cdn.net/csz/news/800a/2022/new-astrobiology-resea.jpg</t>
+  </si>
+  <si>
+    <t>Testing updation</t>
+  </si>
+  <si>
     <t>New astrobiology research predicts life 'as we don't know it'</t>
   </si>
   <si>
-    <t>https://scx1.b-cdn.net/csz/news/800a/2022/new-astrobiology-resea.jpg</t>
-  </si>
-  <si>
     <t>The search for alien life has been restricted to using life on Earth as the reference, essentially looking for "life as we know it" beyond Earth. For astrobiologists looking for life on other planets, there are simply no tools for predicting the features of "life as we don't know it."</t>
   </si>
   <si>
@@ -81,6 +93,12 @@
     <t>A team of researchers affiliated with several institutions in China and one in Austria has confirmed that a circular mountain ridge in China's Heilongjiang Province is a crater made by an asteroid strike. In their paper published in the journal Meteoritics &amp; Planetary Science, the group describes their study of the crater and what they learned about it.</t>
   </si>
   <si>
+    <t>Crescent shaped</t>
+  </si>
+  <si>
+    <t>Post updated</t>
+  </si>
+  <si>
     <t>A rocket is going to crash into the moon: Accidental experiment on the physics of impacts in space</t>
   </si>
   <si>
@@ -126,7 +144,7 @@
     <t>GOES-T was transported from Astrotech's Space Operations facility in Titusville, Florida, to United Launch Alliance's (ULA) nearby Vertical Integration Facility at Cape Canaveral Space Force Station's Space Launch Complex 41. It was then mated to the top of the Atlas V 541 rocket, which will carry it into space. Liftoff is targeted for March 1, 2022, at 4:38 p.m.</t>
   </si>
   <si>
-    <t>The brightest planets in March's night sky: How to see them (and when)</t>
+    <t>The brightest planets in March's night sky</t>
   </si>
   <si>
     <t>https://cdn.mos.cms.futurecdn.net/A6D5yFtvAqub97YAWAJXvM-970-80.jpg</t>
@@ -139,7 +157,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -154,6 +172,10 @@
       <color rgb="FF0000FF"/>
     </font>
     <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <b/>
       <color rgb="FF212438"/>
       <name val="Quicksand"/>
@@ -166,6 +188,10 @@
       <sz val="15.0"/>
       <color rgb="FF212438"/>
       <name val="Quicksand"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
     <font>
       <u/>
@@ -189,18 +215,19 @@
       <color rgb="FF333333"/>
       <name val="&quot;Open Sans&quot;"/>
     </font>
-    <font>
-      <sz val="15.0"/>
-      <color rgb="FF000000"/>
-      <name val="Quicksand"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -215,41 +242,51 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,7 +514,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -485,150 +522,208 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B6" s="4">
+        <v>1234.0</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
+      <c r="B9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="5" t="s">
+      <c r="C10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="D10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="7" t="s">
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="5" t="s">
+      <c r="B11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D11" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="5" t="s">
+      <c r="E11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="F11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="7" t="s">
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="5" t="s">
+      <c r="B12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="6" t="s">
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="B13" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="5" t="s">
+      <c r="C13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="D13" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="E13" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="5" t="s">
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B14" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C14" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="5" t="s">
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C15" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="5" t="s">
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B16" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C16" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="10" t="s">
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B17" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="C15" s="12"/>
-    </row>
-    <row r="16" ht="15.75" customHeight="1"/>
-    <row r="17" ht="15.75" customHeight="1"/>
-    <row r="18" ht="15.75" customHeight="1"/>
-    <row r="19" ht="15.75" customHeight="1"/>
-    <row r="20" ht="15.75" customHeight="1"/>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="8"/>
+      <c r="C20" s="16"/>
+    </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
     <row r="23" ht="15.75" customHeight="1"/>
@@ -1609,21 +1704,28 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
+    <row r="1003" ht="15.75" customHeight="1"/>
+    <row r="1004" ht="15.75" customHeight="1"/>
+    <row r="1005" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B5"/>
-    <hyperlink r:id="rId2" ref="B6"/>
-    <hyperlink r:id="rId3" ref="B7"/>
-    <hyperlink r:id="rId4" ref="B8"/>
-    <hyperlink r:id="rId5" ref="B9"/>
-    <hyperlink r:id="rId6" ref="C9"/>
-    <hyperlink r:id="rId7" ref="B10"/>
-    <hyperlink r:id="rId8" ref="B11"/>
-    <hyperlink r:id="rId9" ref="B12"/>
-    <hyperlink r:id="rId10" ref="B13"/>
-    <hyperlink r:id="rId11" ref="C13"/>
-    <hyperlink r:id="rId12" ref="B14"/>
+    <hyperlink r:id="rId1" ref="B10"/>
+    <hyperlink r:id="rId2" ref="B11"/>
+    <hyperlink r:id="rId3" ref="E11"/>
+    <hyperlink r:id="rId4" ref="B12"/>
+    <hyperlink r:id="rId5" ref="B13"/>
+    <hyperlink r:id="rId6" ref="E13"/>
+    <hyperlink r:id="rId7" ref="B14"/>
+    <hyperlink r:id="rId8" ref="C14"/>
+    <hyperlink r:id="rId9" ref="B15"/>
+    <hyperlink r:id="rId10" ref="B16"/>
+    <hyperlink r:id="rId11" ref="B17"/>
+    <hyperlink r:id="rId12" ref="B18"/>
+    <hyperlink r:id="rId13" ref="C18"/>
+    <hyperlink r:id="rId14" ref="B19"/>
   </hyperlinks>
-  <drawing r:id="rId13"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added test navigation of admin and  trainer page
</commit_message>
<xml_diff>
--- a/IctakTechBlog/src/main/resources/TestData.xlsx
+++ b/IctakTechBlog/src/main/resources/TestData.xlsx
@@ -3,20 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Trainer" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Admin" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhzZ7keGwLMdW9VgM8sHuWi1OCJXw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mgQxvccHylAtn/eyZGmy8UcJAqnMQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
   <si>
     <t>trainerict@gmail.com</t>
   </si>
@@ -151,13 +152,52 @@
   </si>
   <si>
     <t>Mercury is approaching the sun and is a difficult object for mid-northern observers. On the first day of the month, about a half hour before sunrise, look for the zero-magnitude planet very close to the east-southeast horizon, 22 degrees to Venus' lower left.</t>
+  </si>
+  <si>
+    <t>admin2</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>post</t>
+  </si>
+  <si>
+    <t>WEB APPLICATIONS</t>
+  </si>
+  <si>
+    <t>SDS</t>
+  </si>
+  <si>
+    <t>In computer system, a web application is a client-side and server-side software application in which the client runs or request in a web browser.</t>
+  </si>
+  <si>
+    <t>Jblava@gmail.com</t>
+  </si>
+  <si>
+    <t>Lavanya123</t>
+  </si>
+  <si>
+    <t>MOB APPLICATIONS</t>
+  </si>
+  <si>
+    <t>BDS</t>
+  </si>
+  <si>
+    <t>Mobile Web applications refer to applications for mobile devices that require only a Web browser to be installed on the device.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="12">
+  <fonts count="16">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -215,6 +255,27 @@
       <color rgb="FF333333"/>
       <name val="&quot;Open Sans&quot;"/>
     </font>
+    <font>
+      <sz val="8.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <color rgb="FF18191B"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8.0"/>
+      <color rgb="FF6B006D"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8.0"/>
+      <color rgb="FF18191B"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -236,13 +297,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF9A9A9A"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF9A9A9A"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF9A9A9A"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9A9A9A"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -288,6 +363,21 @@
     <xf borderId="0" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -297,6 +387,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1728,4 +1822,143 @@
   </hyperlinks>
   <drawing r:id="rId15"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="73.86"/>
+    <col customWidth="1" min="3" max="3" width="96.57"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="17">
+        <v>1234.0</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="17">
+        <v>12342.0</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="17">
+        <v>12345.0</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="17">
+        <v>1234.0</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="A5"/>
+    <hyperlink r:id="rId2" ref="B9"/>
+    <hyperlink r:id="rId3" ref="C9"/>
+    <hyperlink r:id="rId4" ref="B10"/>
+  </hyperlinks>
+  <drawing r:id="rId5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added test case to update post by Admin
</commit_message>
<xml_diff>
--- a/IctakTechBlog/src/main/resources/TestData.xlsx
+++ b/IctakTechBlog/src/main/resources/TestData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
   <si>
     <t>trainerict@gmail.com</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Testnavya1234</t>
+  </si>
+  <si>
+    <t>Krishna Priya</t>
   </si>
   <si>
     <t>Priya</t>
@@ -663,155 +666,155 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
@@ -1850,7 +1853,7 @@
     </row>
     <row r="2">
       <c r="A2" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B2" s="17">
         <v>12342.0</v>
@@ -1860,54 +1863,54 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C4" s="17">
         <v>1.0</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C6" s="17">
         <v>1.0</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7">
@@ -1922,7 +1925,7 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="17">
         <v>1234.0</v>
@@ -1932,24 +1935,24 @@
     </row>
     <row r="9">
       <c r="A9" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>